<commit_message>
fix: even occur error, markdown was re-written
</commit_message>
<xml_diff>
--- a/doc/Book1.xlsx
+++ b/doc/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryo\PlainTextProject\backup-via-Git\vscode-note-taking-extension\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F165F1-AF1B-4E44-ADE1-F375FD26CA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D42A44-AED8-4EE0-A210-5B6DEC394324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="23040" windowWidth="27000" windowHeight="12255" activeTab="1" xr2:uid="{F0C5EEC0-42B8-40FD-9E09-7FC8049A7E3D}"/>
+    <workbookView xWindow="4710" yWindow="5580" windowWidth="27000" windowHeight="12255" activeTab="2" xr2:uid="{F0C5EEC0-42B8-40FD-9E09-7FC8049A7E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Lion" sheetId="1" r:id="rId1"/>
     <sheet name="Japan" sheetId="2" r:id="rId2"/>
+    <sheet name="Screenshot" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>Q=70</t>
   </si>
@@ -209,6 +210,65 @@
     <t>767.77 KB
 (786,194 bytes)</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>166.84 KB
+(170,846 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PNG</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>92.34 KB
+(94,556 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>109 KB
+(111,618 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>144.01 KB
+(147,462 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>211.52 KB
+(216,596 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>44.04 KB
+(45,094 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>159.44 KB
+(163,267 bytes)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>41.52 KB
+(42,520 bytes)</t>
+  </si>
+  <si>
+    <t>37.37 KB
+(38,267 bytes)</t>
+  </si>
+  <si>
+    <t>48.96 KB
+(50,131 bytes)</t>
+  </si>
+  <si>
+    <t>56.46 KB
+(57,816 bytes)</t>
+  </si>
+  <si>
+    <t>100.5 KB
+(102,907 bytes)</t>
   </si>
 </sst>
 </file>
@@ -734,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45F8ABD-1B8E-4983-86DB-A2C715FEB0C1}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -882,4 +942,158 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8348A2DE-3799-48C2-A06F-A53796EB179C}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.5" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="20.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="37.5" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>